<commit_message>
resultados tras segundo test
</commit_message>
<xml_diff>
--- a/salidaaerodinamicapeq.xlsx
+++ b/salidaaerodinamicapeq.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\verti\Desktop\misilnl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{32A9691F-8959-401A-9C19-9FAF98157CD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75E59953-DA8A-4048-B1D2-D5E2FC180764}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{3332A07A-3A53-4694-9487-9424BCCB03D5}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="baseline1" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" fullCalcOnLoad="true"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,10 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
-  <si>
-    <t>Tiempo</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
   <si>
     <t>Fx</t>
   </si>
@@ -55,6 +53,132 @@
   </si>
   <si>
     <t>N</t>
+  </si>
+  <si>
+    <t>time</t>
+  </si>
+  <si>
+    <t>(3)</t>
+  </si>
+  <si>
+    <t>AbsTol: 0</t>
+  </si>
+  <si>
+    <t>BlockPath: Misil_Simulink_Harness1/Aerodinamicaa</t>
+  </si>
+  <si>
+    <t>Source: Output</t>
+  </si>
+  <si>
+    <t>(5)</t>
+  </si>
+  <si>
+    <t>(6)</t>
+  </si>
+  <si>
+    <t>(3)</t>
+  </si>
+  <si>
+    <t>AbsTol: 0</t>
+  </si>
+  <si>
+    <t>BlockPath: Misil_Simulink_Harness1/Out1</t>
+  </si>
+  <si>
+    <t>Interp: zoh</t>
+  </si>
+  <si>
+    <t>(5)</t>
+  </si>
+  <si>
+    <t>(6)</t>
+  </si>
+  <si>
+    <t>Time</t>
+  </si>
+  <si>
+    <t>time</t>
+  </si>
+  <si>
+    <t>(3)</t>
+  </si>
+  <si>
+    <t>AbsTol: 0</t>
+  </si>
+  <si>
+    <t>BlockPath: Misil_Simulink_Harness1/Aerodinamicaa</t>
+  </si>
+  <si>
+    <t>Source: Output</t>
+  </si>
+  <si>
+    <t>(5)</t>
+  </si>
+  <si>
+    <t>(6)</t>
+  </si>
+  <si>
+    <t>(3)</t>
+  </si>
+  <si>
+    <t>AbsTol: 0</t>
+  </si>
+  <si>
+    <t>BlockPath: Misil_Simulink_Harness1/Out1</t>
+  </si>
+  <si>
+    <t>Interp: zoh</t>
+  </si>
+  <si>
+    <t>(5)</t>
+  </si>
+  <si>
+    <t>(6)</t>
+  </si>
+  <si>
+    <t>time</t>
+  </si>
+  <si>
+    <t>(1)</t>
+  </si>
+  <si>
+    <t>AbsTol: 0</t>
+  </si>
+  <si>
+    <t>BlockPath: Misil_Simulink_Harness1/Aerodinamicaa</t>
+  </si>
+  <si>
+    <t>Source: Output</t>
+  </si>
+  <si>
+    <t>(3)</t>
+  </si>
+  <si>
+    <t>(5)</t>
+  </si>
+  <si>
+    <t>(6)</t>
+  </si>
+  <si>
+    <t>(1)</t>
+  </si>
+  <si>
+    <t>AbsTol: 0</t>
+  </si>
+  <si>
+    <t>BlockPath: Misil_Simulink_Harness1/Out1</t>
+  </si>
+  <si>
+    <t>Interp: zoh</t>
+  </si>
+  <si>
+    <t>(3)</t>
+  </si>
+  <si>
+    <t>(5)</t>
+  </si>
+  <si>
+    <t>(6)</t>
   </si>
 </sst>
 </file>
@@ -78,7 +202,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -86,13 +210,25 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -409,36 +545,36 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05BAA382-2551-42C3-97B4-FD5EEB0C2B86}">
   <dimension ref="A1:G52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A52" sqref="A52:G52"/>
+    <sheetView tabSelected="true" workbookViewId="0">
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>0</v>
       </c>
@@ -461,7 +597,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>0.2</v>
       </c>
@@ -484,7 +620,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>0.4</v>
       </c>
@@ -507,7 +643,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>0.6</v>
       </c>
@@ -530,7 +666,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>0.8</v>
       </c>
@@ -553,7 +689,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>1</v>
       </c>
@@ -576,7 +712,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>1.2</v>
       </c>
@@ -599,7 +735,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>1.4</v>
       </c>
@@ -622,7 +758,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>1.6</v>
       </c>
@@ -645,7 +781,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>1.8</v>
       </c>
@@ -668,7 +804,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>2</v>
       </c>
@@ -691,7 +827,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>2.2000000000000002</v>
       </c>
@@ -714,7 +850,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>2.4</v>
       </c>
@@ -737,7 +873,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>2.6</v>
       </c>
@@ -760,7 +896,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>2.8</v>
       </c>
@@ -783,7 +919,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>3</v>
       </c>
@@ -806,7 +942,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>3.2</v>
       </c>
@@ -829,7 +965,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>3.4</v>
       </c>
@@ -852,7 +988,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="20" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>3.6</v>
       </c>
@@ -875,7 +1011,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="21" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>3.8</v>
       </c>
@@ -898,7 +1034,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="22" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>4</v>
       </c>
@@ -921,7 +1057,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="23" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>4.2</v>
       </c>
@@ -944,7 +1080,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="24" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>4.4000000000000004</v>
       </c>
@@ -967,7 +1103,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="25" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>4.5999999999999996</v>
       </c>
@@ -990,7 +1126,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="26" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>4.8</v>
       </c>
@@ -1013,7 +1149,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="27" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>5</v>
       </c>
@@ -1036,7 +1172,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="28" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>5.2</v>
       </c>
@@ -1059,7 +1195,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="29" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>5.4</v>
       </c>
@@ -1082,7 +1218,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="30" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>5.6</v>
       </c>
@@ -1105,7 +1241,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="31" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>5.8</v>
       </c>
@@ -1128,7 +1264,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="32" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>6</v>
       </c>
@@ -1151,7 +1287,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="33" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>6.2</v>
       </c>
@@ -1174,7 +1310,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="34" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>6.4</v>
       </c>
@@ -1197,7 +1333,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="35" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>6.6</v>
       </c>
@@ -1220,7 +1356,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="36" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>6.8</v>
       </c>
@@ -1243,7 +1379,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="37" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>7</v>
       </c>
@@ -1266,7 +1402,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="38" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>7.2</v>
       </c>
@@ -1289,7 +1425,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="39" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>7.4</v>
       </c>
@@ -1312,7 +1448,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="40" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>7.6</v>
       </c>
@@ -1335,7 +1471,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="41" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>7.8</v>
       </c>
@@ -1358,7 +1494,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="42" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>8</v>
       </c>
@@ -1381,7 +1517,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="43" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>8.1999999999999993</v>
       </c>
@@ -1404,7 +1540,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="44" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>8.4</v>
       </c>
@@ -1427,7 +1563,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="45" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>8.6</v>
       </c>
@@ -1450,7 +1586,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="46" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>8.8000000000000007</v>
       </c>
@@ -1473,7 +1609,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="47" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>9</v>
       </c>
@@ -1496,7 +1632,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="48" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>9.1999999999999993</v>
       </c>
@@ -1519,7 +1655,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="49" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>9.4</v>
       </c>
@@ -1542,7 +1678,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="50" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>9.6</v>
       </c>
@@ -1565,7 +1701,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="51" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>9.8000000000000007</v>
       </c>
@@ -1588,7 +1724,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="52" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>10</v>
       </c>
@@ -1609,6 +1745,1594 @@
       </c>
       <c r="G52">
         <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:I56"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="4.82421875" customWidth="true"/>
+    <col min="2" max="2" width="43.15625" customWidth="true"/>
+    <col min="3" max="3" width="3.26953125" customWidth="true"/>
+    <col min="5" max="5" width="3.26953125" customWidth="true"/>
+    <col min="6" max="6" width="34.93359375" customWidth="true"/>
+    <col min="4" max="4" width="3.26953125" customWidth="true"/>
+    <col min="7" max="7" width="3.26953125" customWidth="true"/>
+    <col min="8" max="8" width="3.26953125" customWidth="true"/>
+    <col min="9" max="9" width="3.26953125" customWidth="true"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="H1" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="I1" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="0"/>
+      <c r="B2" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2" s="0"/>
+      <c r="D2" s="0"/>
+      <c r="E2" s="0"/>
+      <c r="F2" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="G2" s="0"/>
+      <c r="H2" s="0"/>
+      <c r="I2" s="0"/>
+    </row>
+    <row r="3">
+      <c r="A3" s="0"/>
+      <c r="B3" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="C3" s="0"/>
+      <c r="D3" s="0"/>
+      <c r="E3" s="0"/>
+      <c r="F3" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="G3" s="0"/>
+      <c r="H3" s="0"/>
+      <c r="I3" s="0"/>
+    </row>
+    <row r="4">
+      <c r="A4" s="0"/>
+      <c r="B4" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="C4" s="0"/>
+      <c r="D4" s="0"/>
+      <c r="E4" s="0"/>
+      <c r="F4" s="0"/>
+      <c r="G4" s="0"/>
+      <c r="H4" s="0"/>
+      <c r="I4" s="0"/>
+    </row>
+    <row r="5">
+      <c r="A5" s="0"/>
+      <c r="B5" s="0"/>
+      <c r="C5" s="0"/>
+      <c r="D5" s="0"/>
+      <c r="E5" s="0"/>
+      <c r="F5" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="G5" s="0"/>
+      <c r="H5" s="0"/>
+      <c r="I5" s="0"/>
+    </row>
+    <row r="6">
+      <c r="A6" s="0">
+        <v>0</v>
+      </c>
+      <c r="B6" s="0">
+        <v>1895.984769253547</v>
+      </c>
+      <c r="C6" s="0">
+        <v>104.01523072053335</v>
+      </c>
+      <c r="D6" s="0">
+        <v>-0</v>
+      </c>
+      <c r="E6" s="0">
+        <v>-0</v>
+      </c>
+      <c r="F6" s="0">
+        <v>1895.984769253547</v>
+      </c>
+      <c r="G6" s="0">
+        <v>104.01523072053335</v>
+      </c>
+      <c r="H6" s="0">
+        <v>-0</v>
+      </c>
+      <c r="I6" s="0">
+        <v>-0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="0">
+        <v>0.20000000000000001</v>
+      </c>
+      <c r="B7" s="0">
+        <v>1888.7992825359356</v>
+      </c>
+      <c r="C7" s="0">
+        <v>81.937099328847623</v>
+      </c>
+      <c r="D7" s="0">
+        <v>6.110585945471259e-05</v>
+      </c>
+      <c r="E7" s="0">
+        <v>-0</v>
+      </c>
+      <c r="F7" s="0">
+        <v>1888.7992825359356</v>
+      </c>
+      <c r="G7" s="0">
+        <v>81.937099328847623</v>
+      </c>
+      <c r="H7" s="0">
+        <v>6.110585945471259e-05</v>
+      </c>
+      <c r="I7" s="0">
+        <v>-0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="0">
+        <v>0.40000000000000002</v>
+      </c>
+      <c r="B8" s="0">
+        <v>1868.0815951334775</v>
+      </c>
+      <c r="C8" s="0">
+        <v>26.611249035473776</v>
+      </c>
+      <c r="D8" s="0">
+        <v>0.00037709187712757269</v>
+      </c>
+      <c r="E8" s="0">
+        <v>-0</v>
+      </c>
+      <c r="F8" s="0">
+        <v>1868.0815951334775</v>
+      </c>
+      <c r="G8" s="0">
+        <v>26.611249035473776</v>
+      </c>
+      <c r="H8" s="0">
+        <v>0.00037709187712757269</v>
+      </c>
+      <c r="I8" s="0">
+        <v>-0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="0">
+        <v>0.60000000000000009</v>
+      </c>
+      <c r="B9" s="0">
+        <v>1835.3286834671324</v>
+      </c>
+      <c r="C9" s="0">
+        <v>-37.34939806177448</v>
+      </c>
+      <c r="D9" s="0">
+        <v>0.00043531394529175129</v>
+      </c>
+      <c r="E9" s="0">
+        <v>-0</v>
+      </c>
+      <c r="F9" s="0">
+        <v>1835.3286834671324</v>
+      </c>
+      <c r="G9" s="0">
+        <v>-37.34939806177448</v>
+      </c>
+      <c r="H9" s="0">
+        <v>0.00043531394529175129</v>
+      </c>
+      <c r="I9" s="0">
+        <v>-0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="0">
+        <v>0.80000000000000004</v>
+      </c>
+      <c r="B10" s="0">
+        <v>1791.3033435435004</v>
+      </c>
+      <c r="C10" s="0">
+        <v>-87.53358290051078</v>
+      </c>
+      <c r="D10" s="0">
+        <v>0.00030244212289602093</v>
+      </c>
+      <c r="E10" s="0">
+        <v>-0</v>
+      </c>
+      <c r="F10" s="0">
+        <v>1791.3033435435004</v>
+      </c>
+      <c r="G10" s="0">
+        <v>-87.53358290051078</v>
+      </c>
+      <c r="H10" s="0">
+        <v>0.00030244212289602093</v>
+      </c>
+      <c r="I10" s="0">
+        <v>-0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="0">
+        <v>1</v>
+      </c>
+      <c r="B11" s="0">
+        <v>1736.2050563618172</v>
+      </c>
+      <c r="C11" s="0">
+        <v>-113.97476189713534</v>
+      </c>
+      <c r="D11" s="0">
+        <v>-0.0019293849331178505</v>
+      </c>
+      <c r="E11" s="0">
+        <v>-0</v>
+      </c>
+      <c r="F11" s="0">
+        <v>1736.2050563618172</v>
+      </c>
+      <c r="G11" s="0">
+        <v>-113.97476189713534</v>
+      </c>
+      <c r="H11" s="0">
+        <v>-0.0019293849331178505</v>
+      </c>
+      <c r="I11" s="0">
+        <v>-0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="0">
+        <v>1.2000000000000002</v>
+      </c>
+      <c r="B12" s="0">
+        <v>1670.7038691826729</v>
+      </c>
+      <c r="C12" s="0">
+        <v>-119.09070674181936</v>
+      </c>
+      <c r="D12" s="0">
+        <v>0.00018310608211998347</v>
+      </c>
+      <c r="E12" s="0">
+        <v>-0</v>
+      </c>
+      <c r="F12" s="0">
+        <v>1670.7038691826729</v>
+      </c>
+      <c r="G12" s="0">
+        <v>-119.09070674181936</v>
+      </c>
+      <c r="H12" s="0">
+        <v>0.00018310608211998347</v>
+      </c>
+      <c r="I12" s="0">
+        <v>-0</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="0">
+        <v>1.4000000000000001</v>
+      </c>
+      <c r="B13" s="0">
+        <v>1596.3507192725942</v>
+      </c>
+      <c r="C13" s="0">
+        <v>-111.33957816206996</v>
+      </c>
+      <c r="D13" s="0">
+        <v>-0.00050874865488541483</v>
+      </c>
+      <c r="E13" s="0">
+        <v>-0</v>
+      </c>
+      <c r="F13" s="0">
+        <v>1596.3507192725942</v>
+      </c>
+      <c r="G13" s="0">
+        <v>-111.33957816206996</v>
+      </c>
+      <c r="H13" s="0">
+        <v>-0.00050874865488541483</v>
+      </c>
+      <c r="I13" s="0">
+        <v>-0</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="0">
+        <v>1.6000000000000001</v>
+      </c>
+      <c r="B14" s="0">
+        <v>1515.2145318644484</v>
+      </c>
+      <c r="C14" s="0">
+        <v>-98.833448190403971</v>
+      </c>
+      <c r="D14" s="0">
+        <v>-0.00078764823776558148</v>
+      </c>
+      <c r="E14" s="0">
+        <v>-0</v>
+      </c>
+      <c r="F14" s="0">
+        <v>1515.2145318644484</v>
+      </c>
+      <c r="G14" s="0">
+        <v>-98.833448190403971</v>
+      </c>
+      <c r="H14" s="0">
+        <v>-0.00078764823776558148</v>
+      </c>
+      <c r="I14" s="0">
+        <v>-0</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="0">
+        <v>1.8</v>
+      </c>
+      <c r="B15" s="0">
+        <v>1429.3983822333817</v>
+      </c>
+      <c r="C15" s="0">
+        <v>-86.416325728446836</v>
+      </c>
+      <c r="D15" s="0">
+        <v>-0.0001754448611514271</v>
+      </c>
+      <c r="E15" s="0">
+        <v>-0</v>
+      </c>
+      <c r="F15" s="0">
+        <v>1429.3983822333817</v>
+      </c>
+      <c r="G15" s="0">
+        <v>-86.416325728446836</v>
+      </c>
+      <c r="H15" s="0">
+        <v>-0.0001754448611514271</v>
+      </c>
+      <c r="I15" s="0">
+        <v>-0</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="0">
+        <v>2</v>
+      </c>
+      <c r="B16" s="0">
+        <v>1340.7993649119658</v>
+      </c>
+      <c r="C16" s="0">
+        <v>-75.877057420578325</v>
+      </c>
+      <c r="D16" s="0">
+        <v>-0.0014464345336643338</v>
+      </c>
+      <c r="E16" s="0">
+        <v>-0</v>
+      </c>
+      <c r="F16" s="0">
+        <v>1340.7993649119658</v>
+      </c>
+      <c r="G16" s="0">
+        <v>-75.877057420578325</v>
+      </c>
+      <c r="H16" s="0">
+        <v>-0.0014464345336643338</v>
+      </c>
+      <c r="I16" s="0">
+        <v>-0</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="0">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="B17" s="0">
+        <v>1251.0654795244191</v>
+      </c>
+      <c r="C17" s="0">
+        <v>-67.319613117894349</v>
+      </c>
+      <c r="D17" s="0">
+        <v>-0.0019165745937672345</v>
+      </c>
+      <c r="E17" s="0">
+        <v>-0</v>
+      </c>
+      <c r="F17" s="0">
+        <v>1251.0654795244191</v>
+      </c>
+      <c r="G17" s="0">
+        <v>-67.319613117894349</v>
+      </c>
+      <c r="H17" s="0">
+        <v>-0.0019165745937672345</v>
+      </c>
+      <c r="I17" s="0">
+        <v>-0</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="0">
+        <v>2.4000000000000004</v>
+      </c>
+      <c r="B18" s="0">
+        <v>1161.6144755399039</v>
+      </c>
+      <c r="C18" s="0">
+        <v>-60.292586457478066</v>
+      </c>
+      <c r="D18" s="0">
+        <v>-0.0010767123391562548</v>
+      </c>
+      <c r="E18" s="0">
+        <v>-0</v>
+      </c>
+      <c r="F18" s="0">
+        <v>1161.6144755399039</v>
+      </c>
+      <c r="G18" s="0">
+        <v>-60.292586457478066</v>
+      </c>
+      <c r="H18" s="0">
+        <v>-0.0010767123391562548</v>
+      </c>
+      <c r="I18" s="0">
+        <v>-0</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="0">
+        <v>2.6000000000000001</v>
+      </c>
+      <c r="B19" s="0">
+        <v>1073.6502679390835</v>
+      </c>
+      <c r="C19" s="0">
+        <v>-54.335564998993917</v>
+      </c>
+      <c r="D19" s="0">
+        <v>-0.005754767906897911</v>
+      </c>
+      <c r="E19" s="0">
+        <v>-0</v>
+      </c>
+      <c r="F19" s="0">
+        <v>1073.6502679390835</v>
+      </c>
+      <c r="G19" s="0">
+        <v>-54.335564998993917</v>
+      </c>
+      <c r="H19" s="0">
+        <v>-0.005754767906897911</v>
+      </c>
+      <c r="I19" s="0">
+        <v>-0</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="0">
+        <v>2.8000000000000003</v>
+      </c>
+      <c r="B20" s="0">
+        <v>988.16975639583518</v>
+      </c>
+      <c r="C20" s="0">
+        <v>-49.128382972980589</v>
+      </c>
+      <c r="D20" s="0">
+        <v>-0.0015279913935051176</v>
+      </c>
+      <c r="E20" s="0">
+        <v>-0</v>
+      </c>
+      <c r="F20" s="0">
+        <v>988.16975639583518</v>
+      </c>
+      <c r="G20" s="0">
+        <v>-49.128382972980589</v>
+      </c>
+      <c r="H20" s="0">
+        <v>-0.0015279913935051176</v>
+      </c>
+      <c r="I20" s="0">
+        <v>-0</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="0">
+        <v>3</v>
+      </c>
+      <c r="B21" s="0">
+        <v>905.96846618080633</v>
+      </c>
+      <c r="C21" s="0">
+        <v>-44.478318397919963</v>
+      </c>
+      <c r="D21" s="0">
+        <v>-0.0019012374775691809</v>
+      </c>
+      <c r="E21" s="0">
+        <v>-0</v>
+      </c>
+      <c r="F21" s="0">
+        <v>905.96846618080633</v>
+      </c>
+      <c r="G21" s="0">
+        <v>-44.478318397919963</v>
+      </c>
+      <c r="H21" s="0">
+        <v>-0.0019012374775691809</v>
+      </c>
+      <c r="I21" s="0">
+        <v>-0</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="0">
+        <v>3.2000000000000002</v>
+      </c>
+      <c r="B22" s="0">
+        <v>827.65068585640324</v>
+      </c>
+      <c r="C22" s="0">
+        <v>-40.274181754329646</v>
+      </c>
+      <c r="D22" s="0">
+        <v>-0.00088962680101240693</v>
+      </c>
+      <c r="E22" s="0">
+        <v>-0</v>
+      </c>
+      <c r="F22" s="0">
+        <v>827.65068585640324</v>
+      </c>
+      <c r="G22" s="0">
+        <v>-40.274181754329646</v>
+      </c>
+      <c r="H22" s="0">
+        <v>-0.00088962680101240693</v>
+      </c>
+      <c r="I22" s="0">
+        <v>-0</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="0">
+        <v>3.4000000000000004</v>
+      </c>
+      <c r="B23" s="0">
+        <v>753.64508380328198</v>
+      </c>
+      <c r="C23" s="0">
+        <v>-36.449999703291226</v>
+      </c>
+      <c r="D23" s="0">
+        <v>-0.0016842365714812746</v>
+      </c>
+      <c r="E23" s="0">
+        <v>-0</v>
+      </c>
+      <c r="F23" s="0">
+        <v>753.64508380328198</v>
+      </c>
+      <c r="G23" s="0">
+        <v>-36.449999703291226</v>
+      </c>
+      <c r="H23" s="0">
+        <v>-0.0016842365714812746</v>
+      </c>
+      <c r="I23" s="0">
+        <v>-0</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="0">
+        <v>3.6000000000000001</v>
+      </c>
+      <c r="B24" s="0">
+        <v>684.22442586294687</v>
+      </c>
+      <c r="C24" s="0">
+        <v>-32.963387864159969</v>
+      </c>
+      <c r="D24" s="0">
+        <v>-0.0052339344248863743</v>
+      </c>
+      <c r="E24" s="0">
+        <v>-0</v>
+      </c>
+      <c r="F24" s="0">
+        <v>684.22442586294687</v>
+      </c>
+      <c r="G24" s="0">
+        <v>-32.963387864159969</v>
+      </c>
+      <c r="H24" s="0">
+        <v>-0.0052339344248863743</v>
+      </c>
+      <c r="I24" s="0">
+        <v>-0</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="0">
+        <v>3.8000000000000003</v>
+      </c>
+      <c r="B25" s="0">
+        <v>619.52746545593129</v>
+      </c>
+      <c r="C25" s="0">
+        <v>-29.784037640978667</v>
+      </c>
+      <c r="D25" s="0">
+        <v>-0.0044431235649526005</v>
+      </c>
+      <c r="E25" s="0">
+        <v>-0</v>
+      </c>
+      <c r="F25" s="0">
+        <v>619.52746545593129</v>
+      </c>
+      <c r="G25" s="0">
+        <v>-29.784037640978667</v>
+      </c>
+      <c r="H25" s="0">
+        <v>-0.0044431235649526005</v>
+      </c>
+      <c r="I25" s="0">
+        <v>-0</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="0">
+        <v>4</v>
+      </c>
+      <c r="B26" s="0">
+        <v>559.5813034537714</v>
+      </c>
+      <c r="C26" s="0">
+        <v>-26.88783882557793</v>
+      </c>
+      <c r="D26" s="0">
+        <v>-0.011476969704075766</v>
+      </c>
+      <c r="E26" s="0">
+        <v>-0</v>
+      </c>
+      <c r="F26" s="0">
+        <v>559.5813034537714</v>
+      </c>
+      <c r="G26" s="0">
+        <v>-26.88783882557793</v>
+      </c>
+      <c r="H26" s="0">
+        <v>-0.011476969704075766</v>
+      </c>
+      <c r="I26" s="0">
+        <v>-0</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="0">
+        <v>4.2000000000000002</v>
+      </c>
+      <c r="B27" s="0">
+        <v>504.32294475492995</v>
+      </c>
+      <c r="C27" s="0">
+        <v>-24.253939042734473</v>
+      </c>
+      <c r="D27" s="0">
+        <v>-0.001134077236083289</v>
+      </c>
+      <c r="E27" s="0">
+        <v>-0</v>
+      </c>
+      <c r="F27" s="0">
+        <v>504.32294475492995</v>
+      </c>
+      <c r="G27" s="0">
+        <v>-24.253939042734473</v>
+      </c>
+      <c r="H27" s="0">
+        <v>-0.001134077236083289</v>
+      </c>
+      <c r="I27" s="0">
+        <v>-0</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="0">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="B28" s="0">
+        <v>453.6191942383698</v>
+      </c>
+      <c r="C28" s="0">
+        <v>-21.86326322137927</v>
+      </c>
+      <c r="D28" s="0">
+        <v>-0.0044465502553582663</v>
+      </c>
+      <c r="E28" s="0">
+        <v>-0</v>
+      </c>
+      <c r="F28" s="0">
+        <v>453.6191942383698</v>
+      </c>
+      <c r="G28" s="0">
+        <v>-21.86326322137927</v>
+      </c>
+      <c r="H28" s="0">
+        <v>-0.0044465502553582663</v>
+      </c>
+      <c r="I28" s="0">
+        <v>-0</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="0">
+        <v>4.6000000000000005</v>
+      </c>
+      <c r="B29" s="0">
+        <v>407.28439104632702</v>
+      </c>
+      <c r="C29" s="0">
+        <v>-19.69783956014976</v>
+      </c>
+      <c r="D29" s="0">
+        <v>-0.007468338938947639</v>
+      </c>
+      <c r="E29" s="0">
+        <v>-0</v>
+      </c>
+      <c r="F29" s="0">
+        <v>407.28439104632702</v>
+      </c>
+      <c r="G29" s="0">
+        <v>-19.69783956014976</v>
+      </c>
+      <c r="H29" s="0">
+        <v>-0.007468338938947639</v>
+      </c>
+      <c r="I29" s="0">
+        <v>-0</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="0">
+        <v>4.8000000000000007</v>
+      </c>
+      <c r="B30" s="0">
+        <v>365.09574713693581</v>
+      </c>
+      <c r="C30" s="0">
+        <v>-17.740494360157086</v>
+      </c>
+      <c r="D30" s="0">
+        <v>-0.00074925969765881684</v>
+      </c>
+      <c r="E30" s="0">
+        <v>-0</v>
+      </c>
+      <c r="F30" s="0">
+        <v>365.09574713693581</v>
+      </c>
+      <c r="G30" s="0">
+        <v>-17.740494360157086</v>
+      </c>
+      <c r="H30" s="0">
+        <v>-0.00074925969765881684</v>
+      </c>
+      <c r="I30" s="0">
+        <v>-0</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="0">
+        <v>5</v>
+      </c>
+      <c r="B31" s="0">
+        <v>326.80626181467659</v>
+      </c>
+      <c r="C31" s="0">
+        <v>-15.974756311117886</v>
+      </c>
+      <c r="D31" s="0">
+        <v>-0.0010067880427482047</v>
+      </c>
+      <c r="E31" s="0">
+        <v>-0</v>
+      </c>
+      <c r="F31" s="0">
+        <v>326.80626181467659</v>
+      </c>
+      <c r="G31" s="0">
+        <v>-15.974756311117886</v>
+      </c>
+      <c r="H31" s="0">
+        <v>-0.0010067880427482047</v>
+      </c>
+      <c r="I31" s="0">
+        <v>-0</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="0">
+        <v>5.2000000000000002</v>
+      </c>
+      <c r="B32" s="0">
+        <v>292.15532069598964</v>
+      </c>
+      <c r="C32" s="0">
+        <v>-14.384869042614994</v>
+      </c>
+      <c r="D32" s="0">
+        <v>-0.0055041980464403438</v>
+      </c>
+      <c r="E32" s="0">
+        <v>-0</v>
+      </c>
+      <c r="F32" s="0">
+        <v>292.15532069598964</v>
+      </c>
+      <c r="G32" s="0">
+        <v>-14.384869042614994</v>
+      </c>
+      <c r="H32" s="0">
+        <v>-0.0055041980464403438</v>
+      </c>
+      <c r="I32" s="0">
+        <v>-0</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="0">
+        <v>5.4000000000000004</v>
+      </c>
+      <c r="B33" s="0">
+        <v>260.87717311622117</v>
+      </c>
+      <c r="C33" s="0">
+        <v>-12.955832496102857</v>
+      </c>
+      <c r="D33" s="0">
+        <v>-0.001063935167592557</v>
+      </c>
+      <c r="E33" s="0">
+        <v>-0</v>
+      </c>
+      <c r="F33" s="0">
+        <v>260.87717311622117</v>
+      </c>
+      <c r="G33" s="0">
+        <v>-12.955832496102857</v>
+      </c>
+      <c r="H33" s="0">
+        <v>-0.001063935167592557</v>
+      </c>
+      <c r="I33" s="0">
+        <v>-0</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="0">
+        <v>5.6000000000000005</v>
+      </c>
+      <c r="B34" s="0">
+        <v>232.70753017741475</v>
+      </c>
+      <c r="C34" s="0">
+        <v>-11.673447743927625</v>
+      </c>
+      <c r="D34" s="0">
+        <v>-0.00070986351568736469</v>
+      </c>
+      <c r="E34" s="0">
+        <v>-0</v>
+      </c>
+      <c r="F34" s="0">
+        <v>232.70753017741475</v>
+      </c>
+      <c r="G34" s="0">
+        <v>-11.673447743927625</v>
+      </c>
+      <c r="H34" s="0">
+        <v>-0.00070986351568736469</v>
+      </c>
+      <c r="I34" s="0">
+        <v>-0</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="0">
+        <v>5.8000000000000007</v>
+      </c>
+      <c r="B35" s="0">
+        <v>207.38854370885647</v>
+      </c>
+      <c r="C35" s="0">
+        <v>-10.524366584472205</v>
+      </c>
+      <c r="D35" s="0">
+        <v>-0.0010540204777293456</v>
+      </c>
+      <c r="E35" s="0">
+        <v>-0</v>
+      </c>
+      <c r="F35" s="0">
+        <v>207.38854370885647</v>
+      </c>
+      <c r="G35" s="0">
+        <v>-10.524366584472205</v>
+      </c>
+      <c r="H35" s="0">
+        <v>-0.0010540204777293456</v>
+      </c>
+      <c r="I35" s="0">
+        <v>-0</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="0">
+        <v>6</v>
+      </c>
+      <c r="B36" s="0">
+        <v>184.67242161970199</v>
+      </c>
+      <c r="C36" s="0">
+        <v>-9.4961160055862877</v>
+      </c>
+      <c r="D36" s="0">
+        <v>-0.0010588941538630006</v>
+      </c>
+      <c r="E36" s="0">
+        <v>-0</v>
+      </c>
+      <c r="F36" s="0">
+        <v>184.67242161970199</v>
+      </c>
+      <c r="G36" s="0">
+        <v>-9.4961160055862877</v>
+      </c>
+      <c r="H36" s="0">
+        <v>-0.0010588941538630006</v>
+      </c>
+      <c r="I36" s="0">
+        <v>-0</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="0">
+        <v>6.2000000000000002</v>
+      </c>
+      <c r="B37" s="0">
+        <v>164.32392088411444</v>
+      </c>
+      <c r="C37" s="0">
+        <v>-8.5771085840602552</v>
+      </c>
+      <c r="D37" s="0">
+        <v>-0.0045383521621758472</v>
+      </c>
+      <c r="E37" s="0">
+        <v>-0</v>
+      </c>
+      <c r="F37" s="0">
+        <v>164.32392088411444</v>
+      </c>
+      <c r="G37" s="0">
+        <v>-8.5771085840602552</v>
+      </c>
+      <c r="H37" s="0">
+        <v>-0.0045383521621758472</v>
+      </c>
+      <c r="I37" s="0">
+        <v>-0</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="0">
+        <v>6.4000000000000004</v>
+      </c>
+      <c r="B38" s="0">
+        <v>146.12193526842987</v>
+      </c>
+      <c r="C38" s="0">
+        <v>-7.7566393236352127</v>
+      </c>
+      <c r="D38" s="0">
+        <v>-0.0070354666182925957</v>
+      </c>
+      <c r="E38" s="0">
+        <v>-0</v>
+      </c>
+      <c r="F38" s="0">
+        <v>146.12193526842987</v>
+      </c>
+      <c r="G38" s="0">
+        <v>-7.7566393236352127</v>
+      </c>
+      <c r="H38" s="0">
+        <v>-0.0070354666182925957</v>
+      </c>
+      <c r="I38" s="0">
+        <v>-0</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="0">
+        <v>6.6000000000000005</v>
+      </c>
+      <c r="B39" s="0">
+        <v>129.86036769487526</v>
+      </c>
+      <c r="C39" s="0">
+        <v>-7.0248656219873169</v>
+      </c>
+      <c r="D39" s="0">
+        <v>-0.0029361380576351211</v>
+      </c>
+      <c r="E39" s="0">
+        <v>-0</v>
+      </c>
+      <c r="F39" s="0">
+        <v>129.86036769487526</v>
+      </c>
+      <c r="G39" s="0">
+        <v>-7.0248656219873169</v>
+      </c>
+      <c r="H39" s="0">
+        <v>-0.0029361380576351211</v>
+      </c>
+      <c r="I39" s="0">
+        <v>-0</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="0">
+        <v>6.8000000000000007</v>
+      </c>
+      <c r="B40" s="0">
+        <v>115.34844973055415</v>
+      </c>
+      <c r="C40" s="0">
+        <v>-6.3727721738983547</v>
+      </c>
+      <c r="D40" s="0">
+        <v>-0.020369796178753913</v>
+      </c>
+      <c r="E40" s="0">
+        <v>-0</v>
+      </c>
+      <c r="F40" s="0">
+        <v>115.34844973055415</v>
+      </c>
+      <c r="G40" s="0">
+        <v>-6.3727721738983547</v>
+      </c>
+      <c r="H40" s="0">
+        <v>-0.020369796178753913</v>
+      </c>
+      <c r="I40" s="0">
+        <v>-0</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="0">
+        <v>7</v>
+      </c>
+      <c r="B41" s="0">
+        <v>102.41064555784909</v>
+      </c>
+      <c r="C41" s="0">
+        <v>-5.7921502594438437</v>
+      </c>
+      <c r="D41" s="0">
+        <v>-0.0035564732568992251</v>
+      </c>
+      <c r="E41" s="0">
+        <v>-0</v>
+      </c>
+      <c r="F41" s="0">
+        <v>102.41064555784909</v>
+      </c>
+      <c r="G41" s="0">
+        <v>-5.7921502594438437</v>
+      </c>
+      <c r="H41" s="0">
+        <v>-0.0035564732568992251</v>
+      </c>
+      <c r="I41" s="0">
+        <v>-0</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="0">
+        <v>7.2000000000000002</v>
+      </c>
+      <c r="B42" s="0">
+        <v>90.886248857861901</v>
+      </c>
+      <c r="C42" s="0">
+        <v>-5.2755247338420048</v>
+      </c>
+      <c r="D42" s="0">
+        <v>-0.0083639806090725147</v>
+      </c>
+      <c r="E42" s="0">
+        <v>-0</v>
+      </c>
+      <c r="F42" s="0">
+        <v>90.886248857861901</v>
+      </c>
+      <c r="G42" s="0">
+        <v>-5.2755247338420048</v>
+      </c>
+      <c r="H42" s="0">
+        <v>-0.0083639806090725147</v>
+      </c>
+      <c r="I42" s="0">
+        <v>-0</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="0">
+        <v>7.4000000000000004</v>
+      </c>
+      <c r="B43" s="0">
+        <v>80.62876795365311</v>
+      </c>
+      <c r="C43" s="0">
+        <v>-4.8161346693349998</v>
+      </c>
+      <c r="D43" s="0">
+        <v>-0.011793641294456599</v>
+      </c>
+      <c r="E43" s="0">
+        <v>-0</v>
+      </c>
+      <c r="F43" s="0">
+        <v>80.62876795365311</v>
+      </c>
+      <c r="G43" s="0">
+        <v>-4.8161346693349998</v>
+      </c>
+      <c r="H43" s="0">
+        <v>-0.011793641294456599</v>
+      </c>
+      <c r="I43" s="0">
+        <v>-0</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="0">
+        <v>7.6000000000000005</v>
+      </c>
+      <c r="B44" s="0">
+        <v>71.505166131594848</v>
+      </c>
+      <c r="C44" s="0">
+        <v>-4.4078707219199913</v>
+      </c>
+      <c r="D44" s="0">
+        <v>-0.0012220994100759128</v>
+      </c>
+      <c r="E44" s="0">
+        <v>-0</v>
+      </c>
+      <c r="F44" s="0">
+        <v>71.505166131594848</v>
+      </c>
+      <c r="G44" s="0">
+        <v>-4.4078707219199913</v>
+      </c>
+      <c r="H44" s="0">
+        <v>-0.0012220994100759128</v>
+      </c>
+      <c r="I44" s="0">
+        <v>-0</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="0">
+        <v>7.8000000000000007</v>
+      </c>
+      <c r="B45" s="0">
+        <v>63.395015628584858</v>
+      </c>
+      <c r="C45" s="0">
+        <v>-4.0452215973103165</v>
+      </c>
+      <c r="D45" s="0">
+        <v>-0.0011952276151244627</v>
+      </c>
+      <c r="E45" s="0">
+        <v>-0</v>
+      </c>
+      <c r="F45" s="0">
+        <v>63.395015628584858</v>
+      </c>
+      <c r="G45" s="0">
+        <v>-4.0452215973103165</v>
+      </c>
+      <c r="H45" s="0">
+        <v>-0.0011952276151244627</v>
+      </c>
+      <c r="I45" s="0">
+        <v>-0</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="0">
+        <v>8</v>
+      </c>
+      <c r="B46" s="0">
+        <v>56.189608352170254</v>
+      </c>
+      <c r="C46" s="0">
+        <v>-3.7232330115888459</v>
+      </c>
+      <c r="D46" s="0">
+        <v>-0.018913623072687295</v>
+      </c>
+      <c r="E46" s="0">
+        <v>-0</v>
+      </c>
+      <c r="F46" s="0">
+        <v>56.189608352170254</v>
+      </c>
+      <c r="G46" s="0">
+        <v>-3.7232330115888459</v>
+      </c>
+      <c r="H46" s="0">
+        <v>-0.018913623072687295</v>
+      </c>
+      <c r="I46" s="0">
+        <v>-0</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="0">
+        <v>8.2000000000000011</v>
+      </c>
+      <c r="B47" s="0">
+        <v>49.791054918270518</v>
+      </c>
+      <c r="C47" s="0">
+        <v>-3.4374658929924493</v>
+      </c>
+      <c r="D47" s="0">
+        <v>-0.00465357973721796</v>
+      </c>
+      <c r="E47" s="0">
+        <v>-0</v>
+      </c>
+      <c r="F47" s="0">
+        <v>49.791054918270518</v>
+      </c>
+      <c r="G47" s="0">
+        <v>-3.4374658929924493</v>
+      </c>
+      <c r="H47" s="0">
+        <v>-0.00465357973721796</v>
+      </c>
+      <c r="I47" s="0">
+        <v>-0</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="0">
+        <v>8.4000000000000004</v>
+      </c>
+      <c r="B48" s="0">
+        <v>44.111394435277063</v>
+      </c>
+      <c r="C48" s="0">
+        <v>-3.1839292897353886</v>
+      </c>
+      <c r="D48" s="0">
+        <v>-0.0041854504156411208</v>
+      </c>
+      <c r="E48" s="0">
+        <v>-0</v>
+      </c>
+      <c r="F48" s="0">
+        <v>44.111394435277063</v>
+      </c>
+      <c r="G48" s="0">
+        <v>-3.1839292897353886</v>
+      </c>
+      <c r="H48" s="0">
+        <v>-0.0041854504156411208</v>
+      </c>
+      <c r="I48" s="0">
+        <v>-0</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="0">
+        <v>8.5999999999999996</v>
+      </c>
+      <c r="B49" s="0">
+        <v>39.071735356785524</v>
+      </c>
+      <c r="C49" s="0">
+        <v>-2.9590603460581377</v>
+      </c>
+      <c r="D49" s="0">
+        <v>-0.00078082491667308374</v>
+      </c>
+      <c r="E49" s="0">
+        <v>-0</v>
+      </c>
+      <c r="F49" s="0">
+        <v>39.071735356785524</v>
+      </c>
+      <c r="G49" s="0">
+        <v>-2.9590603460581377</v>
+      </c>
+      <c r="H49" s="0">
+        <v>-0.00078082491667308374</v>
+      </c>
+      <c r="I49" s="0">
+        <v>-0</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="0">
+        <v>8.8000000000000007</v>
+      </c>
+      <c r="B50" s="0">
+        <v>34.601434949137527</v>
+      </c>
+      <c r="C50" s="0">
+        <v>-2.7596720877438088</v>
+      </c>
+      <c r="D50" s="0">
+        <v>-0.00096432740033963662</v>
+      </c>
+      <c r="E50" s="0">
+        <v>-0</v>
+      </c>
+      <c r="F50" s="0">
+        <v>34.601434949137527</v>
+      </c>
+      <c r="G50" s="0">
+        <v>-2.7596720877438088</v>
+      </c>
+      <c r="H50" s="0">
+        <v>-0.00096432740033963662</v>
+      </c>
+      <c r="I50" s="0">
+        <v>-0</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="0">
+        <v>9</v>
+      </c>
+      <c r="B51" s="0">
+        <v>39.485134802425009</v>
+      </c>
+      <c r="C51" s="0">
+        <v>-2.5371364196380171</v>
+      </c>
+      <c r="D51" s="0">
+        <v>0.0028183055695620261</v>
+      </c>
+      <c r="E51" s="0">
+        <v>-0</v>
+      </c>
+      <c r="F51" s="0">
+        <v>39.485134802425009</v>
+      </c>
+      <c r="G51" s="0">
+        <v>-2.5371364196380171</v>
+      </c>
+      <c r="H51" s="0">
+        <v>0.0028183055695620261</v>
+      </c>
+      <c r="I51" s="0">
+        <v>-0</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="0">
+        <v>9.2000000000000011</v>
+      </c>
+      <c r="B52" s="0">
+        <v>45.22463804877853</v>
+      </c>
+      <c r="C52" s="0">
+        <v>-2.7151320456631112</v>
+      </c>
+      <c r="D52" s="0">
+        <v>0.00097595936298286348</v>
+      </c>
+      <c r="E52" s="0">
+        <v>-0</v>
+      </c>
+      <c r="F52" s="0">
+        <v>45.22463804877853</v>
+      </c>
+      <c r="G52" s="0">
+        <v>-2.7151320456631112</v>
+      </c>
+      <c r="H52" s="0">
+        <v>0.00097595936298286348</v>
+      </c>
+      <c r="I52" s="0">
+        <v>-0</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="0">
+        <v>9.4000000000000004</v>
+      </c>
+      <c r="B53" s="0">
+        <v>50.338787197020011</v>
+      </c>
+      <c r="C53" s="0">
+        <v>-2.9331504403357513</v>
+      </c>
+      <c r="D53" s="0">
+        <v>0.011079305822333005</v>
+      </c>
+      <c r="E53" s="0">
+        <v>-0</v>
+      </c>
+      <c r="F53" s="0">
+        <v>50.338787197020011</v>
+      </c>
+      <c r="G53" s="0">
+        <v>-2.9331504403357513</v>
+      </c>
+      <c r="H53" s="0">
+        <v>0.011079305822333005</v>
+      </c>
+      <c r="I53" s="0">
+        <v>-0</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="0">
+        <v>9.6000000000000014</v>
+      </c>
+      <c r="B54" s="0">
+        <v>54.904394992545178</v>
+      </c>
+      <c r="C54" s="0">
+        <v>-3.1352823408533794</v>
+      </c>
+      <c r="D54" s="0">
+        <v>0.0012166126039848248</v>
+      </c>
+      <c r="E54" s="0">
+        <v>-0</v>
+      </c>
+      <c r="F54" s="0">
+        <v>54.904394992545178</v>
+      </c>
+      <c r="G54" s="0">
+        <v>-3.1352823408533794</v>
+      </c>
+      <c r="H54" s="0">
+        <v>0.0012166126039848248</v>
+      </c>
+      <c r="I54" s="0">
+        <v>-0</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="0">
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="B55" s="0">
+        <v>58.990654740476103</v>
+      </c>
+      <c r="C55" s="0">
+        <v>-3.3171427024103224</v>
+      </c>
+      <c r="D55" s="0">
+        <v>0.0040929045280930559</v>
+      </c>
+      <c r="E55" s="0">
+        <v>-0</v>
+      </c>
+      <c r="F55" s="0">
+        <v>58.990654740476103</v>
+      </c>
+      <c r="G55" s="0">
+        <v>-3.3171427024103224</v>
+      </c>
+      <c r="H55" s="0">
+        <v>0.0040929045280930559</v>
+      </c>
+      <c r="I55" s="0">
+        <v>-0</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="0">
+        <v>10</v>
+      </c>
+      <c r="B56" s="0">
+        <v>62.658053856303141</v>
+      </c>
+      <c r="C56" s="0">
+        <v>-3.4804648678193075</v>
+      </c>
+      <c r="D56" s="0">
+        <v>0.00067361593329452762</v>
+      </c>
+      <c r="E56" s="0">
+        <v>-0</v>
+      </c>
+      <c r="F56" s="0">
+        <v>62.658053856303141</v>
+      </c>
+      <c r="G56" s="0">
+        <v>-3.4804648678193075</v>
+      </c>
+      <c r="H56" s="0">
+        <v>0.00067361593329452762</v>
+      </c>
+      <c r="I56" s="0">
+        <v>-0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>